<commit_message>
Update vessel activity mapping in functions.py
</commit_message>
<xml_diff>
--- a/Complete_code/CORAL/results/Emissions/25 GW (CC)_emissions.xlsx
+++ b/Complete_code/CORAL/results/Emissions/25 GW (CC)_emissions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>HLV</t>
+          <t>Onshore</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,14 +480,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>450177.5</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4.808692224</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2164765.04366976</v>
-      </c>
+        <v>25368.5</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>25 GW (CC)</t>
@@ -500,23 +496,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>HLV</t>
+          <t>Onshore</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Transit</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>11088</v>
-      </c>
-      <c r="E3" t="n">
-        <v>14.875224448</v>
-      </c>
-      <c r="F3" t="n">
-        <v>164936.488679424</v>
-      </c>
+        <v>424809</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>25 GW (CC)</t>
@@ -529,23 +521,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Towing Group</t>
+          <t>Onshore</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Idle at port</t>
+          <t>Transit</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>672579.5244204547</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.407310331</v>
-      </c>
-      <c r="F4" t="n">
-        <v>273948.588715518</v>
-      </c>
+        <v>11088</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>25 GW (CC)</t>
@@ -563,17 +551,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Idle at sea</t>
+          <t>Idle at port</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>108108</v>
+        <v>672579.5244204547</v>
       </c>
       <c r="E5" t="n">
-        <v>0.203655165</v>
+        <v>0.407310331</v>
       </c>
       <c r="F5" t="n">
-        <v>22016.75257782</v>
+        <v>273948.588715518</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -592,17 +580,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Maneuvering</t>
+          <t>Idle at sea</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8316</v>
+        <v>108108</v>
       </c>
       <c r="E6" t="n">
-        <v>2.698858249</v>
+        <v>0.203655165</v>
       </c>
       <c r="F6" t="n">
-        <v>22443.705198684</v>
+        <v>22016.75257782</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -621,19 +609,48 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Maneuvering</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>8316</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.698858249</v>
+      </c>
+      <c r="F7" t="n">
+        <v>22443.705198684</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>25 GW (CC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Towing Group</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Transit</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>72408.375</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E8" t="n">
         <v>4.753093345</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F8" t="n">
         <v>344163.7653347644</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>25 GW (CC)</t>
         </is>

</xml_diff>